<commit_message>
feat: update for A3a cards
</commit_message>
<xml_diff>
--- a/correspondences.xlsx
+++ b/correspondences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathy\Desktop\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A5D0B9-00A0-4185-9D41-22DFCCA8A0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363488B3-06F3-49AA-BC21-8CB5876F19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="8496" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="0" windowWidth="10656" windowHeight="12336" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="A2a" sheetId="5" r:id="rId4"/>
     <sheet name="A2b" sheetId="6" r:id="rId5"/>
     <sheet name="A3" sheetId="7" r:id="rId6"/>
+    <sheet name="A3a" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="1001">
   <si>
     <t>cTR_10</t>
   </si>
@@ -2832,6 +2833,207 @@
   </si>
   <si>
     <t>cPK_10_002510_00_FLORGES</t>
+  </si>
+  <si>
+    <t>PK_10_007250_00</t>
+  </si>
+  <si>
+    <t>Kartana</t>
+  </si>
+  <si>
+    <t>Blacephalon</t>
+  </si>
+  <si>
+    <t>PK_10_007260_00</t>
+  </si>
+  <si>
+    <t>PK_10_007491_00</t>
+  </si>
+  <si>
+    <t>PK_10_007492_00</t>
+  </si>
+  <si>
+    <t>Tapu Koko Ex</t>
+  </si>
+  <si>
+    <t>Xurkitree</t>
+  </si>
+  <si>
+    <t>Zeraora</t>
+  </si>
+  <si>
+    <t>PK_10_007420_00</t>
+  </si>
+  <si>
+    <t>PK_10_007270_00</t>
+  </si>
+  <si>
+    <t>PK_10_007410_00</t>
+  </si>
+  <si>
+    <t>PK_10_007581_00</t>
+  </si>
+  <si>
+    <t>PK_10_007582_00</t>
+  </si>
+  <si>
+    <t>PK_10_007583_00</t>
+  </si>
+  <si>
+    <t>Poipole</t>
+  </si>
+  <si>
+    <t>PK_10_007370_00</t>
+  </si>
+  <si>
+    <t>PK_10_007801_00</t>
+  </si>
+  <si>
+    <t>PK_10_007300_00</t>
+  </si>
+  <si>
+    <t>Stakataka</t>
+  </si>
+  <si>
+    <t>PK_10_007881_00</t>
+  </si>
+  <si>
+    <t>PK_10_007910_00</t>
+  </si>
+  <si>
+    <t>Stufful</t>
+  </si>
+  <si>
+    <t>PK_10_007380_00</t>
+  </si>
+  <si>
+    <t>[Full Art] - Rowlet</t>
+  </si>
+  <si>
+    <t>[Full Art] - Pheromosa</t>
+  </si>
+  <si>
+    <t>[Full Art] - Blacephalon</t>
+  </si>
+  <si>
+    <t>[Full Art] - Alolan Meowth</t>
+  </si>
+  <si>
+    <t>[Full Art] - Silvally</t>
+  </si>
+  <si>
+    <t>[Full Art] - Celesteela</t>
+  </si>
+  <si>
+    <t>[Full Art] - Tapu Koko Ex</t>
+  </si>
+  <si>
+    <t>[Full Art] - Alolan Dugtrio Ex</t>
+  </si>
+  <si>
+    <t>[Full Art] - Guzzlord Ex</t>
+  </si>
+  <si>
+    <t>[Full Art] - Lycanroc Ex</t>
+  </si>
+  <si>
+    <t>[Full Art] - Buzzwole Ex</t>
+  </si>
+  <si>
+    <t>[Immersive] - Buzzwole Ex</t>
+  </si>
+  <si>
+    <t>[Rainbow] - Alolan Dugtrio Ex</t>
+  </si>
+  <si>
+    <t>[Rainbow] - Guzzlord Ex</t>
+  </si>
+  <si>
+    <t>[Rainbow] - Lycanroc Ex</t>
+  </si>
+  <si>
+    <t>[Rainbow] - Tapu Koko Ex</t>
+  </si>
+  <si>
+    <t>[Shiny] - Arcanine Ex</t>
+  </si>
+  <si>
+    <t>[Shiny] - Celebi Ex</t>
+  </si>
+  <si>
+    <t>[Shiny] - Aerodactyl Ex</t>
+  </si>
+  <si>
+    <t>[Shiny] - Pidgeot Ex</t>
+  </si>
+  <si>
+    <t>[Gold] - Nihilego</t>
+  </si>
+  <si>
+    <t>PK_20_007490_00</t>
+  </si>
+  <si>
+    <t>PK_20_007450_00</t>
+  </si>
+  <si>
+    <t>PK_20_007260_00</t>
+  </si>
+  <si>
+    <t>PK_20_007740_00</t>
+  </si>
+  <si>
+    <t>PK_20_007950_00</t>
+  </si>
+  <si>
+    <t>PK_20_007960_00</t>
+  </si>
+  <si>
+    <t>PK_20_007480_00</t>
+  </si>
+  <si>
+    <t>PK_20_007420_00</t>
+  </si>
+  <si>
+    <t>PK_20_007700_00</t>
+  </si>
+  <si>
+    <t>PK_20_007800_00</t>
+  </si>
+  <si>
+    <t>PK_20_007830_00</t>
+  </si>
+  <si>
+    <t>PK_20_007420_01</t>
+  </si>
+  <si>
+    <t>PK_20_007700_01</t>
+  </si>
+  <si>
+    <t>PK_20_007800_01</t>
+  </si>
+  <si>
+    <t>PK_20_007830_01</t>
+  </si>
+  <si>
+    <t>PK_20_007480_01</t>
+  </si>
+  <si>
+    <t>PK_20_007790_00</t>
+  </si>
+  <si>
+    <t>PK_20_002170_02</t>
+  </si>
+  <si>
+    <t>PK_20_000410_01</t>
+  </si>
+  <si>
+    <t>PK_20_002590_02</t>
+  </si>
+  <si>
+    <t>PK_20_002720_01</t>
+  </si>
+  <si>
+    <t>PK_27_000010_00</t>
   </si>
 </sst>
 </file>
@@ -4046,7 +4248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA877BA-079E-4802-B2C8-80779B839614}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -5484,8 +5686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A8222D-5E44-433B-93F3-4227EF9A3A72}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6110,8 +6312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC35FCF9-E1C8-4628-9212-BE95FE242D10}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7147,4 +7349,376 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7899D0-F8D8-4238-8BB8-7972957CAA34}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>935</v>
+      </c>
+      <c r="B3" t="s">
+        <v>934</v>
+      </c>
+      <c r="C3" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B4" t="s">
+        <v>937</v>
+      </c>
+      <c r="C4" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>940</v>
+      </c>
+      <c r="B5" t="s">
+        <v>943</v>
+      </c>
+      <c r="C5" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>941</v>
+      </c>
+      <c r="B6" t="s">
+        <v>944</v>
+      </c>
+      <c r="C6" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>942</v>
+      </c>
+      <c r="B7" t="s">
+        <v>945</v>
+      </c>
+      <c r="C7" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>949</v>
+      </c>
+      <c r="B8" t="s">
+        <v>950</v>
+      </c>
+      <c r="C8" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>953</v>
+      </c>
+      <c r="B9" t="s">
+        <v>952</v>
+      </c>
+      <c r="C9" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>956</v>
+      </c>
+      <c r="B10" t="s">
+        <v>957</v>
+      </c>
+      <c r="C10" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>958</v>
+      </c>
+      <c r="B11" t="s">
+        <v>980</v>
+      </c>
+      <c r="C11" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>959</v>
+      </c>
+      <c r="B12" t="s">
+        <v>979</v>
+      </c>
+      <c r="C12" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>960</v>
+      </c>
+      <c r="B13" t="s">
+        <v>981</v>
+      </c>
+      <c r="C13" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>961</v>
+      </c>
+      <c r="B14" t="s">
+        <v>982</v>
+      </c>
+      <c r="C14" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>962</v>
+      </c>
+      <c r="B15" t="s">
+        <v>983</v>
+      </c>
+      <c r="C15" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>963</v>
+      </c>
+      <c r="B16" t="s">
+        <v>984</v>
+      </c>
+      <c r="C16" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>968</v>
+      </c>
+      <c r="B17" t="s">
+        <v>985</v>
+      </c>
+      <c r="C17" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>964</v>
+      </c>
+      <c r="B18" t="s">
+        <v>986</v>
+      </c>
+      <c r="C18" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>967</v>
+      </c>
+      <c r="B19" t="s">
+        <v>987</v>
+      </c>
+      <c r="C19" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>966</v>
+      </c>
+      <c r="B20" t="s">
+        <v>988</v>
+      </c>
+      <c r="C20" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>965</v>
+      </c>
+      <c r="B21" t="s">
+        <v>989</v>
+      </c>
+      <c r="C21" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>286</v>
+      </c>
+      <c r="B22" t="s">
+        <v>775</v>
+      </c>
+      <c r="C22" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>973</v>
+      </c>
+      <c r="B23" t="s">
+        <v>990</v>
+      </c>
+      <c r="C23" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>972</v>
+      </c>
+      <c r="B24" t="s">
+        <v>991</v>
+      </c>
+      <c r="C24" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>971</v>
+      </c>
+      <c r="B25" t="s">
+        <v>992</v>
+      </c>
+      <c r="C25" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>970</v>
+      </c>
+      <c r="B26" t="s">
+        <v>993</v>
+      </c>
+      <c r="C26" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>969</v>
+      </c>
+      <c r="B27" t="s">
+        <v>994</v>
+      </c>
+      <c r="C27" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>975</v>
+      </c>
+      <c r="B28" t="s">
+        <v>996</v>
+      </c>
+      <c r="C28" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>974</v>
+      </c>
+      <c r="B29" t="s">
+        <v>997</v>
+      </c>
+      <c r="C29" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>976</v>
+      </c>
+      <c r="B30" t="s">
+        <v>998</v>
+      </c>
+      <c r="C30" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>977</v>
+      </c>
+      <c r="B31" t="s">
+        <v>999</v>
+      </c>
+      <c r="C31" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>978</v>
+      </c>
+      <c r="B32" t="s">
+        <v>995</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>